<commit_message>
changed the methodology to calculating the remaining days within python
</commit_message>
<xml_diff>
--- a/email_system/3Dclientelle.xlsx
+++ b/email_system/3Dclientelle.xlsx
@@ -183,10 +183,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.33"/>
@@ -232,7 +232,7 @@
       </c>
       <c r="F2" s="3" t="n">
         <f aca="true">E2-TODAY()</f>
-        <v>-11</v>
+        <v>-38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -254,7 +254,7 @@
       </c>
       <c r="F3" s="3" t="n">
         <f aca="true">E3-TODAY()</f>
-        <v>51</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -276,7 +276,7 @@
       </c>
       <c r="F4" s="3" t="n">
         <f aca="true">E4-TODAY()</f>
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,7 +298,7 @@
       </c>
       <c r="F5" s="3" t="n">
         <f aca="true">E5-TODAY()</f>
-        <v>19</v>
+        <v>-8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working requests of login and logout
</commit_message>
<xml_diff>
--- a/email_system/3Dclientelle.xlsx
+++ b/email_system/3Dclientelle.xlsx
@@ -62,7 +62,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yy"/>
-    <numFmt numFmtId="166" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -183,10 +183,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.33"/>
@@ -232,7 +232,7 @@
       </c>
       <c r="F2" s="3" t="n">
         <f aca="true">E2-TODAY()</f>
-        <v>-38</v>
+        <v>-89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -254,7 +254,7 @@
       </c>
       <c r="F3" s="3" t="n">
         <f aca="true">E3-TODAY()</f>
-        <v>24</v>
+        <v>-27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -265,18 +265,18 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="D4" s="4" t="n">
         <v>44237</v>
       </c>
       <c r="E4" s="4" t="n">
         <f aca="false">D4+C4</f>
-        <v>44297</v>
+        <v>44327</v>
       </c>
       <c r="F4" s="3" t="n">
         <f aca="true">E4-TODAY()</f>
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,7 +298,7 @@
       </c>
       <c r="F5" s="3" t="n">
         <f aca="true">E5-TODAY()</f>
-        <v>-8</v>
+        <v>-59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>